<commit_message>
Updated v0.2.3 prototype Tilty Quad BOM to show reel costs
</commit_message>
<xml_diff>
--- a/Tilty Hardware/Board Files/Tilty Duo:Quad/V0.2.3/BOM.xlsx
+++ b/Tilty Hardware/Board Files/Tilty Duo:Quad/V0.2.3/BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20515"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="28280" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="38400" yWindow="-440" windowWidth="38400" windowHeight="21600" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tilty Duo BT" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="167">
   <si>
     <t>Part</t>
   </si>
@@ -479,6 +479,51 @@
   </si>
   <si>
     <t>22</t>
+  </si>
+  <si>
+    <t>Cost/reel</t>
+  </si>
+  <si>
+    <t>Quantity/reel</t>
+  </si>
+  <si>
+    <t>Cost/part</t>
+  </si>
+  <si>
+    <t>RMCF0603FT10K0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMCF0603FT10K0CT-ND </t>
+  </si>
+  <si>
+    <t>10K Ω 1% Resistor</t>
+  </si>
+  <si>
+    <t>680 Ω 1% Resistor</t>
+  </si>
+  <si>
+    <t>RC1608F681CS</t>
+  </si>
+  <si>
+    <t>LTST-C171KGKT</t>
+  </si>
+  <si>
+    <t>LTST-C170KRKT</t>
+  </si>
+  <si>
+    <t>4Mbit SPI flash memory</t>
+  </si>
+  <si>
+    <t>S25FL204K0TMFI011</t>
+  </si>
+  <si>
+    <t>S25FL204K0TMFI043</t>
+  </si>
+  <si>
+    <t>ERJ-3GEYJ680V</t>
+  </si>
+  <si>
+    <t>8-SOIC</t>
   </si>
 </sst>
 </file>
@@ -576,10 +621,58 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="103">
+  <cellStyleXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -747,7 +840,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="103">
+  <cellStyles count="151">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -800,6 +893,30 @@
     <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
@@ -850,6 +967,30 @@
     <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3883,10 +4024,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q64"/>
+  <dimension ref="A1:U64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3901,9 +4042,10 @@
     <col min="11" max="11" width="13.33203125" customWidth="1"/>
     <col min="12" max="12" width="12.1640625" customWidth="1"/>
     <col min="13" max="13" width="21" customWidth="1"/>
+    <col min="19" max="19" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1">
+    <row r="1" spans="1:21" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3952,8 +4094,17 @@
       <c r="Q1" s="1" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="2" spans="1:17">
+      <c r="S1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -4004,8 +4155,12 @@
         <f>D2*J2</f>
         <v>0.2908</v>
       </c>
-    </row>
-    <row r="3" spans="1:17">
+      <c r="U2" s="15">
+        <f>S2*T2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
       <c r="A3" t="s">
         <v>95</v>
       </c>
@@ -4046,8 +4201,12 @@
         <f>D3*J3</f>
         <v>4.12</v>
       </c>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="U3" s="15">
+        <f t="shared" ref="U3:U28" si="0">S3*T3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -4098,8 +4257,18 @@
         <f>J4*D4</f>
         <v>0.60599999999999998</v>
       </c>
-    </row>
-    <row r="5" spans="1:17">
+      <c r="S4">
+        <v>2500</v>
+      </c>
+      <c r="T4">
+        <v>0.2361</v>
+      </c>
+      <c r="U4" s="15">
+        <f t="shared" si="0"/>
+        <v>590.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -4140,8 +4309,12 @@
         <f>D5*J5</f>
         <v>2.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:17">
+      <c r="U5" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
       <c r="A6" t="s">
         <v>79</v>
       </c>
@@ -4185,8 +4358,12 @@
         <f>D6*J6</f>
         <v>0.59</v>
       </c>
-    </row>
-    <row r="7" spans="1:17">
+      <c r="U6" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
       <c r="A7" t="s">
         <v>85</v>
       </c>
@@ -4237,13 +4414,17 @@
         <f>J7*D7</f>
         <v>2.56</v>
       </c>
-    </row>
-    <row r="8" spans="1:17">
+      <c r="U7" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
       <c r="A8" t="s">
-        <v>136</v>
+        <v>162</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>133</v>
+        <v>166</v>
       </c>
       <c r="C8" t="s">
         <v>134</v>
@@ -4255,48 +4436,59 @@
         <v>19</v>
       </c>
       <c r="F8" t="s">
-        <v>135</v>
+        <v>163</v>
       </c>
       <c r="G8" s="2">
-        <v>0.28999999999999998</v>
+        <v>0.25</v>
       </c>
       <c r="H8" s="2">
-        <v>0.24</v>
+        <v>0.24099999999999999</v>
       </c>
       <c r="I8" s="2">
-        <v>0.23</v>
+        <v>0.24099999999999999</v>
       </c>
       <c r="J8" s="2">
-        <v>0.23</v>
+        <v>0.22259999999999999</v>
       </c>
       <c r="K8" s="2">
-        <v>0.22</v>
+        <v>0.19769999999999999</v>
       </c>
       <c r="L8" t="s">
         <v>46</v>
       </c>
       <c r="M8" s="38" t="s">
-        <v>135</v>
+        <v>164</v>
       </c>
       <c r="N8" s="17">
-        <v>0.22</v>
+        <v>0.20480000000000001</v>
       </c>
       <c r="O8" s="10">
-        <v>3000</v>
+        <v>3600</v>
       </c>
       <c r="P8" s="18"/>
       <c r="Q8" s="15">
         <f>J8*D8</f>
-        <v>0.23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17">
+        <v>0.22259999999999999</v>
+      </c>
+      <c r="S8">
+        <v>3600</v>
+      </c>
+      <c r="T8">
+        <v>0.20480000000000001</v>
+      </c>
+      <c r="U8" s="15">
+        <f t="shared" si="0"/>
+        <v>737.28000000000009</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
       <c r="B9" s="16"/>
       <c r="O9" s="10"/>
       <c r="P9" s="18"/>
       <c r="Q9" s="15"/>
-    </row>
-    <row r="10" spans="1:17">
+      <c r="U9" s="15"/>
+    </row>
+    <row r="10" spans="1:21">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -4340,8 +4532,12 @@
         <f>D10*J10</f>
         <v>4.6639999999999997</v>
       </c>
-    </row>
-    <row r="11" spans="1:17">
+      <c r="U10" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -4385,8 +4581,12 @@
         <f>J11*D11</f>
         <v>0.18360000000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:17">
+      <c r="U11" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -4427,8 +4627,12 @@
         <f>D12*J12</f>
         <v>0.54059999999999997</v>
       </c>
-    </row>
-    <row r="13" spans="1:17">
+      <c r="U12" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
       <c r="B13" s="16"/>
       <c r="D13" s="5"/>
       <c r="G13" s="2"/>
@@ -4439,8 +4643,9 @@
       <c r="O13" s="10"/>
       <c r="P13" s="18"/>
       <c r="Q13" s="15"/>
-    </row>
-    <row r="14" spans="1:17">
+      <c r="U13" s="15"/>
+    </row>
+    <row r="14" spans="1:21">
       <c r="A14" t="s">
         <v>123</v>
       </c>
@@ -4490,8 +4695,18 @@
         <f>D14*J14</f>
         <v>0.27700000000000002</v>
       </c>
-    </row>
-    <row r="15" spans="1:17">
+      <c r="S14">
+        <v>3000</v>
+      </c>
+      <c r="T14">
+        <v>3.9899999999999998E-2</v>
+      </c>
+      <c r="U14" s="15">
+        <f t="shared" si="0"/>
+        <v>119.69999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -4524,14 +4739,30 @@
       </c>
       <c r="K15" s="2">
         <v>0.14580000000000001</v>
+      </c>
+      <c r="L15" t="s">
+        <v>46</v>
+      </c>
+      <c r="M15" t="s">
+        <v>160</v>
       </c>
       <c r="O15" s="10"/>
       <c r="Q15" s="15">
         <f>D15*J15</f>
         <v>0.26700000000000002</v>
       </c>
-    </row>
-    <row r="16" spans="1:17">
+      <c r="S15">
+        <v>6000</v>
+      </c>
+      <c r="T15">
+        <v>3.7600000000000001E-2</v>
+      </c>
+      <c r="U15" s="15">
+        <f t="shared" si="0"/>
+        <v>225.60000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21">
       <c r="A16" t="s">
         <v>64</v>
       </c>
@@ -4564,20 +4795,37 @@
       </c>
       <c r="K16" s="2">
         <v>0.1431</v>
+      </c>
+      <c r="L16" t="s">
+        <v>46</v>
+      </c>
+      <c r="M16" t="s">
+        <v>161</v>
       </c>
       <c r="O16" s="10"/>
       <c r="Q16" s="15">
         <f>D16*J16</f>
         <v>0.24299999999999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:17">
+      <c r="S16">
+        <v>3000</v>
+      </c>
+      <c r="T16">
+        <v>4.2299999999999997E-2</v>
+      </c>
+      <c r="U16" s="15">
+        <f t="shared" si="0"/>
+        <v>126.89999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21">
       <c r="B17" s="16"/>
       <c r="O17" s="10"/>
       <c r="P17" s="18"/>
       <c r="Q17" s="15"/>
-    </row>
-    <row r="18" spans="1:17">
+      <c r="U17" s="15"/>
+    </row>
+    <row r="18" spans="1:21">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -4602,10 +4850,14 @@
       <c r="O18" s="10"/>
       <c r="P18" s="18"/>
       <c r="Q18" s="15"/>
-    </row>
-    <row r="19" spans="1:17">
+      <c r="U18" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21">
       <c r="A19" t="s">
-        <v>129</v>
+        <v>50</v>
       </c>
       <c r="B19" s="24" t="s">
         <v>43</v>
@@ -4654,10 +4906,20 @@
         <f>D19*J19</f>
         <v>2.0799999999999999E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:17">
+      <c r="S19">
+        <v>5000</v>
+      </c>
+      <c r="T19">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="U19" s="15">
+        <f t="shared" si="0"/>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>157</v>
       </c>
       <c r="B20" s="24" t="s">
         <v>43</v>
@@ -4672,7 +4934,7 @@
         <v>19</v>
       </c>
       <c r="F20" t="s">
-        <v>54</v>
+        <v>156</v>
       </c>
       <c r="G20" s="2">
         <v>0.02</v>
@@ -4693,10 +4955,10 @@
         <v>46</v>
       </c>
       <c r="M20" t="s">
-        <v>63</v>
+        <v>155</v>
       </c>
       <c r="N20" s="11">
-        <v>1.6000000000000001E-3</v>
+        <v>2.2000000000000001E-3</v>
       </c>
       <c r="O20" s="10">
         <v>5000</v>
@@ -4706,8 +4968,18 @@
         <f>J20*D20</f>
         <v>1.84E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:17">
+      <c r="S20">
+        <v>5000</v>
+      </c>
+      <c r="T20">
+        <v>2.2000000000000001E-3</v>
+      </c>
+      <c r="U20" s="15">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21">
       <c r="A21" t="s">
         <v>130</v>
       </c>
@@ -4741,14 +5013,37 @@
       <c r="K21" s="2">
         <v>4.7999999999999996E-3</v>
       </c>
-      <c r="N21" s="11"/>
-      <c r="O21" s="10"/>
+      <c r="L21" t="s">
+        <v>46</v>
+      </c>
+      <c r="M21" t="s">
+        <v>165</v>
+      </c>
+      <c r="N21" s="11">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="O21" s="10">
+        <v>5000</v>
+      </c>
       <c r="P21" s="18"/>
-      <c r="Q21" s="15"/>
-    </row>
-    <row r="22" spans="1:17">
+      <c r="Q21" s="15">
+        <f>D21*J21</f>
+        <v>1.6E-2</v>
+      </c>
+      <c r="S21">
+        <v>5000</v>
+      </c>
+      <c r="T21">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="U21" s="15">
+        <f t="shared" si="0"/>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21">
       <c r="A22" t="s">
-        <v>61</v>
+        <v>158</v>
       </c>
       <c r="B22" s="24" t="s">
         <v>43</v>
@@ -4763,7 +5058,7 @@
         <v>19</v>
       </c>
       <c r="F22" t="s">
-        <v>62</v>
+        <v>159</v>
       </c>
       <c r="G22" s="2">
         <v>0.02</v>
@@ -4784,10 +5079,10 @@
         <v>46</v>
       </c>
       <c r="M22" t="s">
-        <v>62</v>
+        <v>159</v>
       </c>
       <c r="N22" s="11">
-        <v>1.6000000000000001E-3</v>
+        <v>1.2999999999999999E-3</v>
       </c>
       <c r="O22" s="10">
         <v>5000</v>
@@ -4797,14 +5092,25 @@
         <f>D22*J22</f>
         <v>9.1999999999999998E-3</v>
       </c>
-    </row>
-    <row r="23" spans="1:17">
+      <c r="S22">
+        <v>5000</v>
+      </c>
+      <c r="T22">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="U22" s="15">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21">
       <c r="B23" s="16"/>
       <c r="O23" s="10"/>
       <c r="P23" s="18"/>
       <c r="Q23" s="15"/>
-    </row>
-    <row r="24" spans="1:17">
+      <c r="U23" s="15"/>
+    </row>
+    <row r="24" spans="1:21">
       <c r="A24" t="s">
         <v>71</v>
       </c>
@@ -4855,8 +5161,18 @@
         <f>D24*J24</f>
         <v>1.5599999999999999E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:17">
+      <c r="S24">
+        <v>4000</v>
+      </c>
+      <c r="T24">
+        <v>2.0999999999999999E-3</v>
+      </c>
+      <c r="U24" s="15">
+        <f t="shared" si="0"/>
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21">
       <c r="A25" t="s">
         <v>68</v>
       </c>
@@ -4907,8 +5223,18 @@
         <f>D25*J25</f>
         <v>5.1000000000000004E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:17">
+      <c r="S25">
+        <v>15000</v>
+      </c>
+      <c r="T25">
+        <v>1.4E-3</v>
+      </c>
+      <c r="U25" s="15">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21">
       <c r="A26" t="s">
         <v>76</v>
       </c>
@@ -4959,8 +5285,18 @@
         <f>J26*D26</f>
         <v>0.186</v>
       </c>
-    </row>
-    <row r="27" spans="1:17">
+      <c r="S26">
+        <v>4000</v>
+      </c>
+      <c r="T26">
+        <v>9.1999999999999998E-3</v>
+      </c>
+      <c r="U26" s="15">
+        <f t="shared" si="0"/>
+        <v>36.799999999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21">
       <c r="A27" t="s">
         <v>90</v>
       </c>
@@ -5011,8 +5347,18 @@
         <f>D27*J27</f>
         <v>1.8599999999999998E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:17">
+      <c r="S27">
+        <v>4000</v>
+      </c>
+      <c r="T27">
+        <v>4.1999999999999997E-3</v>
+      </c>
+      <c r="U27" s="15">
+        <f t="shared" si="0"/>
+        <v>16.8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21">
       <c r="A28" t="s">
         <v>91</v>
       </c>
@@ -5063,8 +5409,18 @@
         <f>D28*J28</f>
         <v>4.02E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:17">
+      <c r="S28">
+        <v>4000</v>
+      </c>
+      <c r="T28">
+        <v>1.1299999999999999E-2</v>
+      </c>
+      <c r="U28" s="15">
+        <f t="shared" si="0"/>
+        <v>45.199999999999996</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21">
       <c r="B29" s="9"/>
       <c r="D29" s="5"/>
       <c r="G29" s="2"/>
@@ -5074,18 +5430,22 @@
       <c r="N29" s="11"/>
       <c r="O29" s="10"/>
     </row>
-    <row r="30" spans="1:17">
+    <row r="30" spans="1:21">
       <c r="B30" s="9"/>
       <c r="Q30" s="15">
         <f>SUM(Q2:Q28)</f>
-        <v>17.431799999999996</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
+        <v>17.440399999999993</v>
+      </c>
+      <c r="U30" s="15">
+        <f>SUM(U2:U28)</f>
+        <v>1956.4300000000005</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21">
       <c r="B31" s="9"/>
       <c r="L31" s="6"/>
     </row>
-    <row r="32" spans="1:17">
+    <row r="32" spans="1:21">
       <c r="A32" s="25" t="s">
         <v>111</v>
       </c>
@@ -5097,7 +5457,17 @@
       </c>
       <c r="Q32" s="15">
         <f>Q30+17.1</f>
-        <v>34.531799999999997</v>
+        <v>34.540399999999991</v>
+      </c>
+      <c r="S32">
+        <v>175</v>
+      </c>
+      <c r="T32">
+        <v>15.29</v>
+      </c>
+      <c r="U32" s="15">
+        <f>S32+S32*T32+U30</f>
+        <v>4807.18</v>
       </c>
     </row>
     <row r="33" spans="1:17">
@@ -5112,7 +5482,7 @@
       </c>
       <c r="Q33" s="15">
         <f>Q32+18.21</f>
-        <v>52.741799999999998</v>
+        <v>52.750399999999992</v>
       </c>
     </row>
     <row r="34" spans="1:17">
@@ -5417,6 +5787,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <ignoredErrors>
     <ignoredError sqref="B22:B23 B34 B36 B19:B20 B25:B26" numberStoredAsText="1"/>
     <ignoredError sqref="Q26 Q20 Q11 Q4" formula="1"/>

</xml_diff>

<commit_message>
Updated v0.2.3 Tilty Quad BOM to show reel costs
</commit_message>
<xml_diff>
--- a/Tilty Hardware/Board Files/Tilty Duo:Quad/V0.2.3/BOM.xlsx
+++ b/Tilty Hardware/Board Files/Tilty Duo:Quad/V0.2.3/BOM.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="168">
   <si>
     <t>Part</t>
   </si>
@@ -524,6 +524,9 @@
   </si>
   <si>
     <t>8-SOIC</t>
+  </si>
+  <si>
+    <t>1623076-1</t>
   </si>
 </sst>
 </file>
@@ -4027,7 +4030,7 @@
   <dimension ref="A1:U64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T15" sqref="T15"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4846,13 +4849,29 @@
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
-      <c r="N18" s="12"/>
-      <c r="O18" s="10"/>
+      <c r="L18" t="s">
+        <v>46</v>
+      </c>
+      <c r="M18" t="s">
+        <v>167</v>
+      </c>
+      <c r="N18" s="12">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="O18" s="10">
+        <v>5000</v>
+      </c>
       <c r="P18" s="18"/>
       <c r="Q18" s="15"/>
+      <c r="S18">
+        <v>5000</v>
+      </c>
+      <c r="T18">
+        <v>1.6000000000000001E-3</v>
+      </c>
       <c r="U18" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:21">
@@ -5438,7 +5457,7 @@
       </c>
       <c r="U30" s="15">
         <f>SUM(U2:U28)</f>
-        <v>1956.4300000000005</v>
+        <v>1964.4300000000005</v>
       </c>
     </row>
     <row r="31" spans="1:21">
@@ -5467,7 +5486,7 @@
       </c>
       <c r="U32" s="15">
         <f>S32+S32*T32+U30</f>
-        <v>4807.18</v>
+        <v>4815.18</v>
       </c>
     </row>
     <row r="33" spans="1:17">

</xml_diff>

<commit_message>
Updated Tilty Duo/Quad BOM
</commit_message>
<xml_diff>
--- a/Tilty Hardware/Board Files/Tilty Duo:Quad/V0.2.3/BOM.xlsx
+++ b/Tilty Hardware/Board Files/Tilty Duo:Quad/V0.2.3/BOM.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="167">
   <si>
     <t>Part</t>
   </si>
@@ -434,9 +434,6 @@
   </si>
   <si>
     <t>8 Kbit I2C EEPROM</t>
-  </si>
-  <si>
-    <t>C5, C9, C12</t>
   </si>
   <si>
     <t>CL10B224KP8NNNC</t>
@@ -2379,7 +2376,7 @@
     </row>
     <row r="29" spans="1:18">
       <c r="A29" s="39" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B29" s="9"/>
       <c r="D29" s="5"/>
@@ -3736,7 +3733,7 @@
     </row>
     <row r="32" spans="1:18">
       <c r="A32" s="39" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B32" s="9"/>
       <c r="D32" s="5"/>
@@ -4027,10 +4024,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U64"/>
+  <dimension ref="A1:U63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4098,13 +4095,13 @@
         <v>102</v>
       </c>
       <c r="S1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>154</v>
-      </c>
       <c r="U1" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:21">
@@ -4205,7 +4202,7 @@
         <v>4.12</v>
       </c>
       <c r="U3" s="15">
-        <f t="shared" ref="U3:U28" si="0">S3*T3</f>
+        <f t="shared" ref="U3:U27" si="0">S3*T3</f>
         <v>0</v>
       </c>
     </row>
@@ -4424,10 +4421,10 @@
     </row>
     <row r="8" spans="1:21">
       <c r="A8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C8" t="s">
         <v>134</v>
@@ -4439,7 +4436,7 @@
         <v>19</v>
       </c>
       <c r="F8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G8" s="2">
         <v>0.25</v>
@@ -4460,7 +4457,7 @@
         <v>46</v>
       </c>
       <c r="M8" s="38" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="N8" s="17">
         <v>0.20480000000000001</v>
@@ -4747,7 +4744,7 @@
         <v>46</v>
       </c>
       <c r="M15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="O15" s="10"/>
       <c r="Q15" s="15">
@@ -4803,7 +4800,7 @@
         <v>46</v>
       </c>
       <c r="M16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O16" s="10"/>
       <c r="Q16" s="15">
@@ -4853,7 +4850,7 @@
         <v>46</v>
       </c>
       <c r="M18" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N18" s="12">
         <v>1.6000000000000001E-3</v>
@@ -4938,7 +4935,7 @@
     </row>
     <row r="20" spans="1:21">
       <c r="A20" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B20" s="24" t="s">
         <v>43</v>
@@ -4953,7 +4950,7 @@
         <v>19</v>
       </c>
       <c r="F20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G20" s="2">
         <v>0.02</v>
@@ -4974,7 +4971,7 @@
         <v>46</v>
       </c>
       <c r="M20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="N20" s="11">
         <v>2.2000000000000001E-3</v>
@@ -5036,7 +5033,7 @@
         <v>46</v>
       </c>
       <c r="M21" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N21" s="11">
         <v>1.1000000000000001E-3</v>
@@ -5062,7 +5059,7 @@
     </row>
     <row r="22" spans="1:21">
       <c r="A22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B22" s="24" t="s">
         <v>43</v>
@@ -5077,7 +5074,7 @@
         <v>19</v>
       </c>
       <c r="F22" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G22" s="2">
         <v>0.02</v>
@@ -5098,7 +5095,7 @@
         <v>46</v>
       </c>
       <c r="M22" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N22" s="11">
         <v>1.2999999999999999E-3</v>
@@ -5146,7 +5143,7 @@
         <v>19</v>
       </c>
       <c r="F24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G24" s="2">
         <v>0.1</v>
@@ -5167,7 +5164,7 @@
         <v>46</v>
       </c>
       <c r="M24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N24" s="11">
         <v>2.0999999999999999E-3</v>
@@ -5199,7 +5196,7 @@
         <v>43</v>
       </c>
       <c r="C25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D25" s="5">
         <v>5</v>
@@ -5208,7 +5205,7 @@
         <v>19</v>
       </c>
       <c r="F25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G25" s="2">
         <v>0.1</v>
@@ -5229,7 +5226,7 @@
         <v>46</v>
       </c>
       <c r="M25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N25" s="11">
         <v>1.4E-3</v>
@@ -5255,75 +5252,75 @@
     </row>
     <row r="26" spans="1:21">
       <c r="A26" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="B26" s="24" t="s">
         <v>43</v>
       </c>
       <c r="C26" t="s">
-        <v>137</v>
+        <v>89</v>
       </c>
       <c r="D26" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E26" t="s">
         <v>19</v>
       </c>
       <c r="F26" t="s">
-        <v>78</v>
+        <v>137</v>
       </c>
       <c r="G26" s="2">
         <v>0.1</v>
       </c>
       <c r="H26" s="2">
-        <v>6.2E-2</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="I26" s="2">
-        <v>6.2E-2</v>
+        <v>2.4400000000000002E-2</v>
       </c>
       <c r="J26" s="2">
-        <v>6.2E-2</v>
+        <v>1.8599999999999998E-2</v>
       </c>
       <c r="K26" s="2">
-        <v>2.86E-2</v>
+        <v>1.5800000000000002E-2</v>
       </c>
       <c r="L26" t="s">
         <v>46</v>
       </c>
       <c r="M26" t="s">
-        <v>78</v>
+        <v>137</v>
       </c>
       <c r="N26" s="11">
-        <v>9.1999999999999998E-3</v>
+        <v>4.1999999999999997E-3</v>
       </c>
       <c r="O26" s="10">
         <v>4000</v>
       </c>
       <c r="P26" s="18"/>
       <c r="Q26" s="15">
-        <f>J26*D26</f>
-        <v>0.186</v>
+        <f>D26*J26</f>
+        <v>1.8599999999999998E-2</v>
       </c>
       <c r="S26">
         <v>4000</v>
       </c>
       <c r="T26">
-        <v>9.1999999999999998E-3</v>
+        <v>4.1999999999999997E-3</v>
       </c>
       <c r="U26" s="15">
         <f t="shared" si="0"/>
-        <v>36.799999999999997</v>
+        <v>16.8</v>
       </c>
     </row>
     <row r="27" spans="1:21">
       <c r="A27" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B27" s="24" t="s">
         <v>43</v>
       </c>
       <c r="C27" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D27" s="5">
         <v>1</v>
@@ -5338,16 +5335,16 @@
         <v>0.1</v>
       </c>
       <c r="H27" s="2">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="I27" s="2">
+        <v>5.2400000000000002E-2</v>
+      </c>
+      <c r="J27" s="2">
+        <v>4.02E-2</v>
+      </c>
+      <c r="K27" s="2">
         <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="I27" s="2">
-        <v>2.4400000000000002E-2</v>
-      </c>
-      <c r="J27" s="2">
-        <v>1.8599999999999998E-2</v>
-      </c>
-      <c r="K27" s="2">
-        <v>1.5800000000000002E-2</v>
       </c>
       <c r="L27" t="s">
         <v>46</v>
@@ -5356,7 +5353,7 @@
         <v>138</v>
       </c>
       <c r="N27" s="11">
-        <v>4.1999999999999997E-3</v>
+        <v>1.1299999999999999E-2</v>
       </c>
       <c r="O27" s="10">
         <v>4000</v>
@@ -5364,152 +5361,105 @@
       <c r="P27" s="18"/>
       <c r="Q27" s="15">
         <f>D27*J27</f>
-        <v>1.8599999999999998E-2</v>
+        <v>4.02E-2</v>
       </c>
       <c r="S27">
         <v>4000</v>
       </c>
       <c r="T27">
-        <v>4.1999999999999997E-3</v>
+        <v>1.1299999999999999E-2</v>
       </c>
       <c r="U27" s="15">
         <f t="shared" si="0"/>
-        <v>16.8</v>
+        <v>45.199999999999996</v>
       </c>
     </row>
     <row r="28" spans="1:21">
-      <c r="A28" t="s">
-        <v>91</v>
-      </c>
-      <c r="B28" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="C28" t="s">
-        <v>92</v>
-      </c>
-      <c r="D28" s="5">
-        <v>1</v>
-      </c>
-      <c r="E28" t="s">
-        <v>19</v>
-      </c>
-      <c r="F28" t="s">
-        <v>139</v>
-      </c>
-      <c r="G28" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="H28" s="2">
-        <v>7.3999999999999996E-2</v>
-      </c>
-      <c r="I28" s="2">
-        <v>5.2400000000000002E-2</v>
-      </c>
-      <c r="J28" s="2">
-        <v>4.02E-2</v>
-      </c>
-      <c r="K28" s="2">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="L28" t="s">
-        <v>46</v>
-      </c>
-      <c r="M28" t="s">
-        <v>139</v>
-      </c>
-      <c r="N28" s="11">
-        <v>1.1299999999999999E-2</v>
-      </c>
-      <c r="O28" s="10">
-        <v>4000</v>
-      </c>
-      <c r="P28" s="18"/>
-      <c r="Q28" s="15">
-        <f>D28*J28</f>
-        <v>4.02E-2</v>
-      </c>
-      <c r="S28">
-        <v>4000</v>
-      </c>
-      <c r="T28">
-        <v>1.1299999999999999E-2</v>
-      </c>
-      <c r="U28" s="15">
-        <f t="shared" si="0"/>
-        <v>45.199999999999996</v>
-      </c>
+      <c r="B28" s="9"/>
+      <c r="D28" s="5"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="10"/>
     </row>
     <row r="29" spans="1:21">
       <c r="B29" s="9"/>
-      <c r="D29" s="5"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="N29" s="11"/>
-      <c r="O29" s="10"/>
+      <c r="Q29" s="15">
+        <f>SUM(Q2:Q27)</f>
+        <v>17.254399999999993</v>
+      </c>
+      <c r="U29" s="15">
+        <f>SUM(U2:U27)</f>
+        <v>1927.6300000000006</v>
+      </c>
     </row>
     <row r="30" spans="1:21">
       <c r="B30" s="9"/>
-      <c r="Q30" s="15">
-        <f>SUM(Q2:Q28)</f>
-        <v>17.440399999999993</v>
-      </c>
-      <c r="U30" s="15">
-        <f>SUM(U2:U28)</f>
-        <v>1964.4300000000005</v>
-      </c>
+      <c r="L30" s="6"/>
     </row>
     <row r="31" spans="1:21">
-      <c r="B31" s="9"/>
-      <c r="L31" s="6"/>
+      <c r="A31" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="B31" s="28">
+        <v>37</v>
+      </c>
+      <c r="P31" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q31" s="15">
+        <f>Q29+17.1</f>
+        <v>34.354399999999998</v>
+      </c>
+      <c r="S31">
+        <v>175</v>
+      </c>
+      <c r="T31">
+        <v>15.29</v>
+      </c>
+      <c r="U31" s="15">
+        <f>S31+S31*T31+U29</f>
+        <v>4778.380000000001</v>
+      </c>
     </row>
     <row r="32" spans="1:21">
       <c r="A32" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="B32" s="28">
-        <v>37</v>
+        <v>112</v>
+      </c>
+      <c r="B32" s="26" t="s">
+        <v>145</v>
       </c>
       <c r="P32" s="9" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="Q32" s="15">
-        <f>Q30+17.1</f>
-        <v>34.540399999999991</v>
-      </c>
-      <c r="S32">
-        <v>175</v>
-      </c>
-      <c r="T32">
-        <v>15.29</v>
-      </c>
-      <c r="U32" s="15">
-        <f>S32+S32*T32+U30</f>
-        <v>4815.18</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17">
+        <f>Q31+18.21</f>
+        <v>52.564399999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
       <c r="A33" s="25" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B33" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="D33" s="5"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="N33" s="11"/>
+      <c r="O33" s="10"/>
+    </row>
+    <row r="34" spans="1:15">
+      <c r="A34" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="B34" s="26" t="s">
         <v>146</v>
-      </c>
-      <c r="P33" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="Q33" s="15">
-        <f>Q32+18.21</f>
-        <v>52.750399999999992</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17">
-      <c r="A34" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="B34" s="26" t="s">
-        <v>116</v>
       </c>
       <c r="D34" s="5"/>
       <c r="G34" s="2"/>
@@ -5519,12 +5469,12 @@
       <c r="N34" s="11"/>
       <c r="O34" s="10"/>
     </row>
-    <row r="35" spans="1:17">
+    <row r="35" spans="1:15">
       <c r="A35" s="25" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>147</v>
+        <v>117</v>
       </c>
       <c r="D35" s="5"/>
       <c r="G35" s="2"/>
@@ -5534,13 +5484,8 @@
       <c r="N35" s="11"/>
       <c r="O35" s="10"/>
     </row>
-    <row r="36" spans="1:17">
-      <c r="A36" s="25" t="s">
-        <v>115</v>
-      </c>
-      <c r="B36" s="26" t="s">
-        <v>117</v>
-      </c>
+    <row r="36" spans="1:15">
+      <c r="B36" s="9"/>
       <c r="D36" s="5"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
@@ -5549,7 +5494,7 @@
       <c r="N36" s="11"/>
       <c r="O36" s="10"/>
     </row>
-    <row r="37" spans="1:17">
+    <row r="37" spans="1:15">
       <c r="B37" s="9"/>
       <c r="D37" s="5"/>
       <c r="G37" s="2"/>
@@ -5559,7 +5504,7 @@
       <c r="N37" s="11"/>
       <c r="O37" s="10"/>
     </row>
-    <row r="38" spans="1:17">
+    <row r="38" spans="1:15">
       <c r="B38" s="9"/>
       <c r="D38" s="5"/>
       <c r="G38" s="2"/>
@@ -5569,7 +5514,7 @@
       <c r="N38" s="11"/>
       <c r="O38" s="10"/>
     </row>
-    <row r="39" spans="1:17">
+    <row r="39" spans="1:15">
       <c r="B39" s="9"/>
       <c r="D39" s="5"/>
       <c r="G39" s="2"/>
@@ -5579,7 +5524,7 @@
       <c r="N39" s="11"/>
       <c r="O39" s="10"/>
     </row>
-    <row r="40" spans="1:17">
+    <row r="40" spans="1:15">
       <c r="B40" s="9"/>
       <c r="D40" s="5"/>
       <c r="G40" s="2"/>
@@ -5589,7 +5534,7 @@
       <c r="N40" s="11"/>
       <c r="O40" s="10"/>
     </row>
-    <row r="41" spans="1:17">
+    <row r="41" spans="1:15">
       <c r="B41" s="9"/>
       <c r="D41" s="5"/>
       <c r="G41" s="2"/>
@@ -5599,7 +5544,7 @@
       <c r="N41" s="11"/>
       <c r="O41" s="10"/>
     </row>
-    <row r="42" spans="1:17">
+    <row r="42" spans="1:15">
       <c r="B42" s="9"/>
       <c r="D42" s="5"/>
       <c r="G42" s="2"/>
@@ -5609,7 +5554,7 @@
       <c r="N42" s="11"/>
       <c r="O42" s="10"/>
     </row>
-    <row r="43" spans="1:17">
+    <row r="43" spans="1:15">
       <c r="B43" s="9"/>
       <c r="D43" s="5"/>
       <c r="G43" s="2"/>
@@ -5619,7 +5564,7 @@
       <c r="N43" s="11"/>
       <c r="O43" s="10"/>
     </row>
-    <row r="44" spans="1:17">
+    <row r="44" spans="1:15">
       <c r="B44" s="9"/>
       <c r="D44" s="5"/>
       <c r="G44" s="2"/>
@@ -5629,7 +5574,7 @@
       <c r="N44" s="11"/>
       <c r="O44" s="10"/>
     </row>
-    <row r="45" spans="1:17">
+    <row r="45" spans="1:15">
       <c r="B45" s="9"/>
       <c r="D45" s="5"/>
       <c r="G45" s="2"/>
@@ -5639,7 +5584,7 @@
       <c r="N45" s="11"/>
       <c r="O45" s="10"/>
     </row>
-    <row r="46" spans="1:17">
+    <row r="46" spans="1:15">
       <c r="B46" s="9"/>
       <c r="D46" s="5"/>
       <c r="G46" s="2"/>
@@ -5649,7 +5594,7 @@
       <c r="N46" s="11"/>
       <c r="O46" s="10"/>
     </row>
-    <row r="47" spans="1:17">
+    <row r="47" spans="1:15">
       <c r="B47" s="9"/>
       <c r="D47" s="5"/>
       <c r="G47" s="2"/>
@@ -5659,7 +5604,7 @@
       <c r="N47" s="11"/>
       <c r="O47" s="10"/>
     </row>
-    <row r="48" spans="1:17">
+    <row r="48" spans="1:15">
       <c r="B48" s="9"/>
       <c r="D48" s="5"/>
       <c r="G48" s="2"/>
@@ -5740,7 +5685,6 @@
       <c r="O55" s="10"/>
     </row>
     <row r="56" spans="2:15">
-      <c r="B56" s="9"/>
       <c r="D56" s="5"/>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
@@ -5755,7 +5699,6 @@
       <c r="H57" s="2"/>
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
-      <c r="N57" s="11"/>
       <c r="O57" s="10"/>
     </row>
     <row r="58" spans="2:15">
@@ -5764,7 +5707,6 @@
       <c r="H58" s="2"/>
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
-      <c r="O58" s="10"/>
     </row>
     <row r="59" spans="2:15">
       <c r="D59" s="5"/>
@@ -5795,21 +5737,14 @@
       <c r="J62" s="2"/>
     </row>
     <row r="63" spans="2:15">
-      <c r="D63" s="5"/>
-      <c r="G63" s="2"/>
-      <c r="H63" s="2"/>
-      <c r="I63" s="2"/>
-      <c r="J63" s="2"/>
-    </row>
-    <row r="64" spans="2:15">
-      <c r="D64" s="3"/>
+      <c r="D63" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <ignoredErrors>
-    <ignoredError sqref="B22:B23 B34 B36 B19:B20 B25:B26" numberStoredAsText="1"/>
-    <ignoredError sqref="Q26 Q20 Q11 Q4" formula="1"/>
-    <ignoredError sqref="Q30" emptyCellReference="1"/>
+    <ignoredError sqref="B22:B23 B33 B35 B19:B20 B25" numberStoredAsText="1"/>
+    <ignoredError sqref="Q20 Q11 Q4" formula="1"/>
+    <ignoredError sqref="Q29" emptyCellReference="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -6635,7 +6570,7 @@
         <v>19</v>
       </c>
       <c r="F21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G21" s="2">
         <v>0.1</v>
@@ -6656,7 +6591,7 @@
         <v>46</v>
       </c>
       <c r="M21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N21" s="11">
         <v>2.0999999999999999E-3</v>
@@ -6678,7 +6613,7 @@
         <v>43</v>
       </c>
       <c r="C22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D22" s="5">
         <v>5</v>
@@ -6687,7 +6622,7 @@
         <v>19</v>
       </c>
       <c r="F22" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G22" s="2">
         <v>0.1</v>
@@ -6708,7 +6643,7 @@
         <v>46</v>
       </c>
       <c r="M22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N22" s="11">
         <v>1.4E-3</v>
@@ -6730,7 +6665,7 @@
         <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D23" s="5">
         <v>2</v>
@@ -6791,7 +6726,7 @@
         <v>19</v>
       </c>
       <c r="F24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G24" s="2">
         <v>0.1</v>
@@ -6812,7 +6747,7 @@
         <v>46</v>
       </c>
       <c r="M24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="N24" s="11">
         <v>4.1999999999999997E-3</v>
@@ -6843,7 +6778,7 @@
         <v>19</v>
       </c>
       <c r="F25" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G25" s="2">
         <v>0.1</v>
@@ -6864,7 +6799,7 @@
         <v>46</v>
       </c>
       <c r="M25" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N25" s="11">
         <v>1.1299999999999999E-2</v>
@@ -6907,7 +6842,7 @@
         <v>31</v>
       </c>
       <c r="P29" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="Q29" s="15">
         <f>Q27+17.1</f>
@@ -6919,10 +6854,10 @@
         <v>112</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="P30" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="Q30" s="15">
         <f>Q29+18.21</f>
@@ -6949,7 +6884,7 @@
         <v>114</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D32" s="5"/>
       <c r="G32" s="2"/>

</xml_diff>